<commit_message>
added PCB render, improved BOM
</commit_message>
<xml_diff>
--- a/KRS-XL.xlsx
+++ b/KRS-XL.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="168">
   <si>
     <t>PCB</t>
   </si>
@@ -67,12 +67,6 @@
     <t>use rest</t>
   </si>
   <si>
-    <t>SMD-Kurzhubtaster, vert. Montage, Höhe 7,0mm</t>
-  </si>
-  <si>
-    <t>TASTER 9316</t>
-  </si>
-  <si>
     <t>Variante</t>
   </si>
   <si>
@@ -355,9 +349,6 @@
     <t>ADUM 1201 AR</t>
   </si>
   <si>
-    <t>JLCPCB</t>
-  </si>
-  <si>
     <t>RND 1206 1 4,7K</t>
   </si>
   <si>
@@ -500,6 +491,42 @@
   </si>
   <si>
     <t>0001</t>
+  </si>
+  <si>
+    <t>0100</t>
+  </si>
+  <si>
+    <t>D1-3</t>
+  </si>
+  <si>
+    <t>BL 1X10G8 2,54</t>
+  </si>
+  <si>
+    <t>1x07 Stiftleiste</t>
+  </si>
+  <si>
+    <t>Stiftleiste 1x7</t>
+  </si>
+  <si>
+    <t>MPE 087-1-007</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>WSL 6G</t>
+  </si>
+  <si>
+    <t>DIM-24CxLED (TFT)</t>
+  </si>
+  <si>
+    <t>MPE 094-1-016</t>
+  </si>
+  <si>
+    <t>MPE 094-1-005</t>
+  </si>
+  <si>
+    <t>MPE 094-1-007</t>
   </si>
 </sst>
 </file>
@@ -869,65 +896,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:Q75"/>
+  <dimension ref="D2:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="47.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="1"/>
     <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.5703125" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" customWidth="1"/>
+    <col min="18" max="18" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H2" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
+      <c r="Q2" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="3" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
         <v>58</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
         <v>59</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" t="s">
         <v>60</v>
       </c>
-      <c r="G3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K3" t="s">
-        <v>62</v>
-      </c>
       <c r="L3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="4:17" x14ac:dyDescent="0.25">
@@ -938,15 +969,21 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>110</v>
+        <v>154</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="J4" s="1">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="M4" s="1"/>
-      <c r="Q4" s="2">
+      <c r="O4" s="2">
         <f>J4*D4</f>
-        <v>2.5</v>
+        <v>4</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="4:17" x14ac:dyDescent="0.25">
@@ -954,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
         <v>1</v>
@@ -963,7 +1000,7 @@
         <v>8</v>
       </c>
       <c r="H5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I5" t="s">
         <v>7</v>
@@ -972,9 +1009,12 @@
         <v>0.15</v>
       </c>
       <c r="M5" s="1"/>
-      <c r="Q5" s="2">
-        <f t="shared" ref="Q5:Q34" si="0">J5*D5</f>
+      <c r="O5" s="2">
+        <f t="shared" ref="O5:O29" si="0">J5*D5</f>
         <v>0.15</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="4:17" x14ac:dyDescent="0.25">
@@ -982,27 +1022,30 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J6" s="1">
         <v>0.12</v>
       </c>
       <c r="M6" s="1"/>
-      <c r="Q6" s="2">
+      <c r="O6" s="2">
         <f t="shared" si="0"/>
         <v>0.12</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="4:17" x14ac:dyDescent="0.25">
@@ -1010,27 +1053,30 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J7" s="1">
         <v>0.12</v>
       </c>
       <c r="M7" s="1"/>
-      <c r="Q7" s="2">
+      <c r="O7" s="2">
         <f t="shared" si="0"/>
         <v>0.12</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="4:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1038,52 +1084,61 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J8" s="1">
         <v>0.12</v>
       </c>
       <c r="M8" s="1"/>
-      <c r="Q8" s="2">
+      <c r="O8" s="2">
         <f t="shared" si="0"/>
         <v>0.12</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="4:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>3</v>
       </c>
+      <c r="E9" t="s">
+        <v>157</v>
+      </c>
       <c r="F9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J9" s="1">
         <v>0.2</v>
       </c>
       <c r="M9" s="1"/>
-      <c r="Q9" s="2">
+      <c r="O9" s="2">
         <f t="shared" si="0"/>
         <v>0.60000000000000009</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="4:17" x14ac:dyDescent="0.25">
@@ -1091,27 +1146,30 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G10" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J10" s="1">
         <v>0.02</v>
       </c>
       <c r="M10" s="1"/>
-      <c r="Q10" s="2">
+      <c r="O10" s="2">
         <f t="shared" si="0"/>
         <v>0.02</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="4:17" x14ac:dyDescent="0.25">
@@ -1119,27 +1177,30 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J11" s="1">
         <v>0.02</v>
       </c>
       <c r="M11" s="1"/>
-      <c r="Q11" s="2">
+      <c r="O11" s="2">
         <f t="shared" si="0"/>
         <v>0.02</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="4:17" x14ac:dyDescent="0.25">
@@ -1147,27 +1208,30 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J12" s="1">
         <v>0.02</v>
       </c>
       <c r="M12" s="1"/>
-      <c r="Q12" s="2">
+      <c r="O12" s="2">
         <f t="shared" si="0"/>
         <v>0.02</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="4:17" x14ac:dyDescent="0.25">
@@ -1175,27 +1239,30 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J13" s="1">
         <v>1.75</v>
       </c>
       <c r="M13" s="1"/>
-      <c r="Q13" s="2">
+      <c r="O13" s="2">
         <f t="shared" si="0"/>
         <v>1.75</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="4:17" x14ac:dyDescent="0.25">
@@ -1203,27 +1270,30 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J14" s="1">
         <v>0.02</v>
       </c>
       <c r="M14" s="1"/>
-      <c r="Q14" s="2">
+      <c r="O14" s="2">
         <f t="shared" si="0"/>
         <v>0.02</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="4:17" x14ac:dyDescent="0.25">
@@ -1231,27 +1301,30 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F15" t="s">
         <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I15" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J15" s="1">
         <v>0.04</v>
       </c>
       <c r="M15" s="1"/>
-      <c r="Q15" s="2">
+      <c r="O15" s="2">
         <f t="shared" si="0"/>
         <v>0.04</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="4:17" x14ac:dyDescent="0.25">
@@ -1259,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F16" t="s">
         <v>11</v>
@@ -1268,18 +1341,21 @@
         <v>9</v>
       </c>
       <c r="H16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J16" s="1">
         <v>0.25</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="Q16" s="2">
+      <c r="O16" s="2">
         <f t="shared" si="0"/>
         <v>0.25</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="4:17" x14ac:dyDescent="0.25">
@@ -1287,27 +1363,30 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F17" t="s">
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J17" s="1">
         <v>0.02</v>
       </c>
       <c r="M17" s="1"/>
-      <c r="Q17" s="2">
+      <c r="O17" s="2">
         <f t="shared" si="0"/>
         <v>0.04</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="4:17" x14ac:dyDescent="0.25">
@@ -1315,27 +1394,30 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J18" s="1">
         <v>10</v>
       </c>
       <c r="M18" s="1"/>
-      <c r="Q18" s="2">
+      <c r="O18" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="4:17" x14ac:dyDescent="0.25">
@@ -1343,18 +1425,30 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G19" t="s">
-        <v>134</v>
+        <v>131</v>
+      </c>
+      <c r="H19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.21</v>
       </c>
       <c r="M19" s="1"/>
-      <c r="Q19" s="2">
+      <c r="O19" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.21</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="4:17" x14ac:dyDescent="0.25">
@@ -1362,27 +1456,30 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>96</v>
+        <v>159</v>
       </c>
       <c r="G20" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="H20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I20" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="J20" s="1">
-        <v>0.03</v>
+        <v>0.16</v>
       </c>
       <c r="M20" s="1"/>
-      <c r="Q20" s="2">
+      <c r="O20" s="2">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.16</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="4:17" x14ac:dyDescent="0.25">
@@ -1393,85 +1490,94 @@
         <v>73</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="G21" t="s">
-        <v>65</v>
+        <v>129</v>
       </c>
       <c r="H21" t="s">
-        <v>145</v>
+        <v>61</v>
       </c>
       <c r="I21" t="s">
+        <v>130</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="M21" s="1"/>
+      <c r="O21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" t="s">
+        <v>142</v>
+      </c>
+      <c r="I22" t="s">
         <v>5</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J22" s="1">
         <v>12.7</v>
       </c>
-      <c r="K21" t="s">
-        <v>146</v>
-      </c>
-      <c r="M21" s="1">
+      <c r="K22" t="s">
+        <v>143</v>
+      </c>
+      <c r="M22" s="1">
         <v>11.84</v>
       </c>
-      <c r="Q21" s="2">
+      <c r="O22" s="2">
         <f t="shared" si="0"/>
         <v>12.7</v>
       </c>
-    </row>
-    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D22">
+      <c r="Q22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D23">
         <v>2</v>
       </c>
-      <c r="E22" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" t="s">
-        <v>135</v>
-      </c>
-      <c r="G22" t="s">
-        <v>140</v>
-      </c>
-      <c r="H22" t="s">
-        <v>63</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" t="s">
+        <v>132</v>
+      </c>
+      <c r="G23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H23" t="s">
+        <v>61</v>
+      </c>
+      <c r="I23" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J23" s="1">
         <v>0.72</v>
       </c>
-      <c r="M22" s="1"/>
-      <c r="Q22" s="2">
+      <c r="M23" s="1"/>
+      <c r="O23" s="2">
         <f t="shared" si="0"/>
         <v>1.44</v>
       </c>
-    </row>
-    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" t="s">
-        <v>136</v>
-      </c>
-      <c r="G23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" t="s">
-        <v>13</v>
-      </c>
-      <c r="J23" s="1">
-        <v>0</v>
-      </c>
-      <c r="M23" s="1"/>
-      <c r="Q23" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="Q23" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="4:17" x14ac:dyDescent="0.25">
@@ -1479,111 +1585,120 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="F24" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="G24" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="H24" t="s">
-        <v>141</v>
+        <v>13</v>
       </c>
       <c r="I24" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="O24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" t="s">
+        <v>138</v>
+      </c>
+      <c r="I25" t="s">
+        <v>139</v>
+      </c>
+      <c r="J25" s="1">
         <v>5.5</v>
       </c>
-      <c r="M24" s="1"/>
-      <c r="Q24" s="2">
+      <c r="M25" s="1"/>
+      <c r="O25" s="2">
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
-    </row>
-    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D25">
+      <c r="Q25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D26">
         <v>4</v>
       </c>
-      <c r="E25" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="E26" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" t="s">
         <v>6</v>
       </c>
-      <c r="G25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" t="s">
-        <v>63</v>
-      </c>
-      <c r="I25" t="s">
-        <v>15</v>
-      </c>
-      <c r="J25" s="1">
+      <c r="G26" t="s">
+        <v>152</v>
+      </c>
+      <c r="H26" t="s">
+        <v>61</v>
+      </c>
+      <c r="I26" t="s">
+        <v>151</v>
+      </c>
+      <c r="J26" s="1">
         <v>0.27</v>
       </c>
-      <c r="M25" s="1"/>
-      <c r="Q25" s="2">
+      <c r="M26" s="1"/>
+      <c r="O26" s="2">
         <f t="shared" si="0"/>
         <v>1.08</v>
       </c>
-    </row>
-    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D26">
+      <c r="Q26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D27">
         <v>2</v>
       </c>
-      <c r="E26" t="s">
-        <v>103</v>
-      </c>
-      <c r="F26" t="s">
-        <v>71</v>
-      </c>
-      <c r="G26" t="s">
-        <v>143</v>
-      </c>
-      <c r="H26" t="s">
-        <v>63</v>
-      </c>
-      <c r="I26" t="s">
-        <v>150</v>
-      </c>
-      <c r="J26" s="1">
+      <c r="E27" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" t="s">
+        <v>140</v>
+      </c>
+      <c r="H27" t="s">
+        <v>61</v>
+      </c>
+      <c r="I27" t="s">
+        <v>147</v>
+      </c>
+      <c r="J27" s="1">
         <v>0.02</v>
       </c>
-      <c r="M26" s="1"/>
-      <c r="Q26" s="2">
+      <c r="M27" s="1"/>
+      <c r="O27" s="2">
         <f t="shared" si="0"/>
         <v>0.04</v>
-      </c>
-    </row>
-    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" t="s">
-        <v>131</v>
-      </c>
-      <c r="H27" t="s">
-        <v>147</v>
-      </c>
-      <c r="I27" t="s">
-        <v>148</v>
-      </c>
-      <c r="J27" s="1">
-        <v>25</v>
-      </c>
-      <c r="M27" s="1"/>
-      <c r="Q27" s="2">
-        <f t="shared" si="0"/>
-        <v>25</v>
       </c>
     </row>
     <row r="28" spans="4:17" x14ac:dyDescent="0.25">
@@ -1591,27 +1706,27 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F28" t="s">
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="G28" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H28" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
       <c r="I28" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="J28" s="1">
-        <v>0.03</v>
+        <v>25</v>
       </c>
       <c r="M28" s="1"/>
-      <c r="Q28" s="2">
+      <c r="O28" s="2">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="4:17" x14ac:dyDescent="0.25">
@@ -1619,248 +1734,276 @@
         <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J29" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="M29" s="1"/>
-      <c r="Q29" s="2">
+      <c r="O29" s="2">
         <f t="shared" si="0"/>
         <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="30" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D30">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F30" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="G30" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="H30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I30" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="J30" s="1">
-        <v>0.02</v>
+        <v>0.2</v>
       </c>
       <c r="M30" s="1"/>
-      <c r="Q30" s="2">
-        <f t="shared" si="0"/>
-        <v>0.06</v>
+      <c r="O30" s="2">
+        <f t="shared" ref="O30" si="1">J30*D30</f>
+        <v>1.6</v>
       </c>
     </row>
     <row r="31" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D31">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F31" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G31" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="H31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I31" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="J31" s="1">
-        <v>0.27</v>
+        <v>0.02</v>
       </c>
       <c r="M31" s="1"/>
-      <c r="Q31" s="2">
-        <f t="shared" si="0"/>
-        <v>2.16</v>
+      <c r="O31" s="2">
+        <f>J31*D31</f>
+        <v>0.06</v>
       </c>
     </row>
     <row r="32" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D32">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F32" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="G32" t="s">
-        <v>85</v>
+        <v>152</v>
       </c>
       <c r="H32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I32" t="s">
-        <v>109</v>
+        <v>151</v>
       </c>
       <c r="J32" s="1">
-        <v>1.7</v>
+        <v>0.27</v>
       </c>
       <c r="M32" s="1"/>
-      <c r="Q32" s="2">
-        <f t="shared" si="0"/>
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="33" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="O32" s="2">
+        <f>J32*D32</f>
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="33" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F33" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G33" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" t="s">
+        <v>61</v>
+      </c>
+      <c r="I33" t="s">
         <v>107</v>
       </c>
-      <c r="H33" t="s">
-        <v>138</v>
-      </c>
-      <c r="I33" t="s">
-        <v>139</v>
-      </c>
       <c r="J33" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="M33" s="1"/>
+      <c r="O33" s="2">
+        <f>J33*D33</f>
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="34" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>85</v>
+      </c>
+      <c r="F34" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" t="s">
+        <v>135</v>
+      </c>
+      <c r="I34" t="s">
+        <v>136</v>
+      </c>
+      <c r="J34" s="1">
         <v>7.03</v>
       </c>
-      <c r="M33" s="1"/>
-      <c r="Q33" s="2">
-        <f t="shared" si="0"/>
+      <c r="M34" s="1"/>
+      <c r="O34" s="2">
+        <f>J34*D34</f>
         <v>7.03</v>
       </c>
     </row>
-    <row r="34" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D34">
+    <row r="35" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D35">
         <v>2</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" t="s">
+        <v>123</v>
+      </c>
+      <c r="G35" t="s">
+        <v>127</v>
+      </c>
+      <c r="H35" t="s">
+        <v>61</v>
+      </c>
+      <c r="I35" t="s">
+        <v>122</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="M35" s="1"/>
+      <c r="O35" s="2">
+        <f>J35*D35</f>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="36" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>72</v>
+      </c>
+      <c r="F36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="O39" s="2">
+        <f>SUM(O4:O38)</f>
+        <v>76.660000000000011</v>
+      </c>
+    </row>
+    <row r="60" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
         <v>74</v>
       </c>
-      <c r="F34" t="s">
-        <v>126</v>
-      </c>
-      <c r="G34" t="s">
-        <v>130</v>
-      </c>
-      <c r="H34" t="s">
-        <v>63</v>
-      </c>
-      <c r="I34" t="s">
-        <v>125</v>
-      </c>
-      <c r="J34" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="M34" s="1"/>
-      <c r="Q34" s="2">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
-        <v>74</v>
-      </c>
-      <c r="F35" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="Q38" s="2">
-        <f>SUM(Q4:Q37)</f>
-        <v>73.220000000000013</v>
-      </c>
-    </row>
-    <row r="59" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E59" t="s">
-        <v>76</v>
-      </c>
-      <c r="F59" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="69" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E69" t="s">
-        <v>79</v>
-      </c>
-      <c r="F69" t="s">
-        <v>78</v>
+      <c r="F60" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F70" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F71" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F72" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F73" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="F74" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="75" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="F75" t="s">
-        <v>88</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="76" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>85</v>
+      </c>
+      <c r="F76" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1892,84 +2035,84 @@
   <sheetData>
     <row r="5" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="O5" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="K6" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="L6" t="s">
         <v>28</v>
       </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" t="s">
-        <v>30</v>
-      </c>
       <c r="M6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="5:17" x14ac:dyDescent="0.25">
@@ -1977,220 +2120,220 @@
         <v>4</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="L7" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="M7" t="s">
         <v>28</v>
       </c>
-      <c r="J7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M7" t="s">
-        <v>30</v>
-      </c>
       <c r="N7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
         <v>28</v>
       </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="4" t="s">
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" t="s">
         <v>28</v>
       </c>
-      <c r="J9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" t="s">
-        <v>30</v>
-      </c>
       <c r="M9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" t="s">
         <v>28</v>
       </c>
-      <c r="G11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" t="s">
-        <v>30</v>
-      </c>
       <c r="K11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="P14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Q14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="P15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>